<commit_message>
March 24 update 3
</commit_message>
<xml_diff>
--- a/Jupyter/simulationID/cim_0324_0620/data/bldg/after_208_12.xlsx
+++ b/Jupyter/simulationID/cim_0324_0620/data/bldg/after_208_12.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="17">
   <si>
     <t>appUnits</t>
   </si>
@@ -49,10 +49,22 @@
     <t>status</t>
   </si>
   <si>
+    <t>renewd</t>
+  </si>
+  <si>
+    <t>PlanID</t>
+  </si>
+  <si>
+    <t>iteration</t>
+  </si>
+  <si>
     <t>208_12</t>
   </si>
   <si>
     <t>Tama 38_1</t>
+  </si>
+  <si>
+    <t>after</t>
   </si>
 </sst>
 </file>
@@ -410,13 +422,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:15">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,8 +462,17 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -459,7 +480,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>97</v>
@@ -486,10 +507,19 @@
         <v>707.3</v>
       </c>
       <c r="L2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2">
+        <v>20181295</v>
+      </c>
+      <c r="O2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -497,7 +527,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>97</v>
@@ -524,10 +554,19 @@
         <v>707.3</v>
       </c>
       <c r="L3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3">
+        <v>20181295</v>
+      </c>
+      <c r="O3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -535,7 +574,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <v>97</v>
@@ -562,10 +601,19 @@
         <v>707.3</v>
       </c>
       <c r="L4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4">
+        <v>20181295</v>
+      </c>
+      <c r="O4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -573,7 +621,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>97</v>
@@ -600,10 +648,19 @@
         <v>707.3</v>
       </c>
       <c r="L5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5">
+        <v>20181295</v>
+      </c>
+      <c r="O5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -611,7 +668,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D6">
         <v>97</v>
@@ -638,10 +695,19 @@
         <v>707.3</v>
       </c>
       <c r="L6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6">
+        <v>20181295</v>
+      </c>
+      <c r="O6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -649,7 +715,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D7">
         <v>97</v>
@@ -676,10 +742,19 @@
         <v>707.3</v>
       </c>
       <c r="L7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7">
+        <v>20181295</v>
+      </c>
+      <c r="O7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -687,7 +762,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <v>97</v>
@@ -714,10 +789,19 @@
         <v>707.3</v>
       </c>
       <c r="L8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8">
+        <v>20181295</v>
+      </c>
+      <c r="O8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -725,7 +809,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D9">
         <v>97</v>
@@ -752,10 +836,19 @@
         <v>707.3</v>
       </c>
       <c r="L9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M9" t="s">
+        <v>16</v>
+      </c>
+      <c r="N9">
+        <v>20181295</v>
+      </c>
+      <c r="O9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -763,7 +856,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D10">
         <v>97</v>
@@ -790,10 +883,19 @@
         <v>707.3</v>
       </c>
       <c r="L10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10">
+        <v>20181295</v>
+      </c>
+      <c r="O10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -801,7 +903,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D11">
         <v>97</v>
@@ -828,10 +930,19 @@
         <v>707.3</v>
       </c>
       <c r="L11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N11">
+        <v>20181295</v>
+      </c>
+      <c r="O11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -839,7 +950,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D12">
         <v>97</v>
@@ -866,10 +977,19 @@
         <v>707.3</v>
       </c>
       <c r="L12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M12" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12">
+        <v>20181295</v>
+      </c>
+      <c r="O12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -877,7 +997,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D13">
         <v>97</v>
@@ -904,10 +1024,19 @@
         <v>707.3</v>
       </c>
       <c r="L13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N13">
+        <v>20181295</v>
+      </c>
+      <c r="O13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -915,7 +1044,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D14">
         <v>97</v>
@@ -942,10 +1071,19 @@
         <v>707.3</v>
       </c>
       <c r="L14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M14" t="s">
+        <v>16</v>
+      </c>
+      <c r="N14">
+        <v>20181295</v>
+      </c>
+      <c r="O14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -953,7 +1091,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D15">
         <v>97</v>
@@ -980,10 +1118,19 @@
         <v>707.3</v>
       </c>
       <c r="L15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M15" t="s">
+        <v>16</v>
+      </c>
+      <c r="N15">
+        <v>20181295</v>
+      </c>
+      <c r="O15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -991,7 +1138,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D16">
         <v>97</v>
@@ -1018,10 +1165,19 @@
         <v>707.3</v>
       </c>
       <c r="L16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M16" t="s">
+        <v>16</v>
+      </c>
+      <c r="N16">
+        <v>20181295</v>
+      </c>
+      <c r="O16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1029,7 +1185,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D17">
         <v>97</v>
@@ -1056,10 +1212,19 @@
         <v>707.3</v>
       </c>
       <c r="L17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N17">
+        <v>20181295</v>
+      </c>
+      <c r="O17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1067,7 +1232,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D18">
         <v>97</v>
@@ -1094,10 +1259,19 @@
         <v>707.3</v>
       </c>
       <c r="L18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M18" t="s">
+        <v>16</v>
+      </c>
+      <c r="N18">
+        <v>20181295</v>
+      </c>
+      <c r="O18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1105,7 +1279,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D19">
         <v>97</v>
@@ -1132,10 +1306,19 @@
         <v>707.3</v>
       </c>
       <c r="L19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M19" t="s">
+        <v>16</v>
+      </c>
+      <c r="N19">
+        <v>20181295</v>
+      </c>
+      <c r="O19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1143,7 +1326,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D20">
         <v>97</v>
@@ -1170,10 +1353,19 @@
         <v>707.3</v>
       </c>
       <c r="L20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M20" t="s">
+        <v>16</v>
+      </c>
+      <c r="N20">
+        <v>20181295</v>
+      </c>
+      <c r="O20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1181,7 +1373,7 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D21">
         <v>97</v>
@@ -1208,10 +1400,19 @@
         <v>707.3</v>
       </c>
       <c r="L21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M21" t="s">
+        <v>16</v>
+      </c>
+      <c r="N21">
+        <v>20181295</v>
+      </c>
+      <c r="O21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1219,7 +1420,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D22">
         <v>97</v>
@@ -1246,10 +1447,19 @@
         <v>707.3</v>
       </c>
       <c r="L22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M22" t="s">
+        <v>16</v>
+      </c>
+      <c r="N22">
+        <v>20181295</v>
+      </c>
+      <c r="O22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1257,7 +1467,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D23">
         <v>97</v>
@@ -1284,10 +1494,19 @@
         <v>707.3</v>
       </c>
       <c r="L23" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M23" t="s">
+        <v>16</v>
+      </c>
+      <c r="N23">
+        <v>20181295</v>
+      </c>
+      <c r="O23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1295,7 +1514,7 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D24">
         <v>97</v>
@@ -1322,10 +1541,19 @@
         <v>707.3</v>
       </c>
       <c r="L24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M24" t="s">
+        <v>16</v>
+      </c>
+      <c r="N24">
+        <v>20181295</v>
+      </c>
+      <c r="O24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1333,7 +1561,7 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D25">
         <v>97</v>
@@ -1360,10 +1588,19 @@
         <v>707.3</v>
       </c>
       <c r="L25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M25" t="s">
+        <v>16</v>
+      </c>
+      <c r="N25">
+        <v>20181295</v>
+      </c>
+      <c r="O25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1371,7 +1608,7 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D26">
         <v>97</v>
@@ -1398,10 +1635,19 @@
         <v>707.3</v>
       </c>
       <c r="L26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M26" t="s">
+        <v>16</v>
+      </c>
+      <c r="N26">
+        <v>20181295</v>
+      </c>
+      <c r="O26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1409,7 +1655,7 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D27">
         <v>97</v>
@@ -1436,10 +1682,19 @@
         <v>707.3</v>
       </c>
       <c r="L27" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M27" t="s">
+        <v>16</v>
+      </c>
+      <c r="N27">
+        <v>20181295</v>
+      </c>
+      <c r="O27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1447,7 +1702,7 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D28">
         <v>97</v>
@@ -1474,10 +1729,19 @@
         <v>707.3</v>
       </c>
       <c r="L28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M28" t="s">
+        <v>16</v>
+      </c>
+      <c r="N28">
+        <v>20181295</v>
+      </c>
+      <c r="O28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1485,7 +1749,7 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D29">
         <v>97</v>
@@ -1512,10 +1776,19 @@
         <v>707.3</v>
       </c>
       <c r="L29" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M29" t="s">
+        <v>16</v>
+      </c>
+      <c r="N29">
+        <v>20181295</v>
+      </c>
+      <c r="O29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1523,7 +1796,7 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D30">
         <v>97</v>
@@ -1550,10 +1823,19 @@
         <v>707.3</v>
       </c>
       <c r="L30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M30" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30">
+        <v>20181295</v>
+      </c>
+      <c r="O30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1561,7 +1843,7 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D31">
         <v>97</v>
@@ -1588,10 +1870,19 @@
         <v>707.3</v>
       </c>
       <c r="L31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M31" t="s">
+        <v>16</v>
+      </c>
+      <c r="N31">
+        <v>20181295</v>
+      </c>
+      <c r="O31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1599,7 +1890,7 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D32">
         <v>97</v>
@@ -1626,10 +1917,19 @@
         <v>707.3</v>
       </c>
       <c r="L32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M32" t="s">
+        <v>16</v>
+      </c>
+      <c r="N32">
+        <v>20181295</v>
+      </c>
+      <c r="O32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1637,7 +1937,7 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D33">
         <v>97</v>
@@ -1664,10 +1964,19 @@
         <v>707.3</v>
       </c>
       <c r="L33" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M33" t="s">
+        <v>16</v>
+      </c>
+      <c r="N33">
+        <v>20181295</v>
+      </c>
+      <c r="O33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1675,7 +1984,7 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D34">
         <v>97</v>
@@ -1702,10 +2011,19 @@
         <v>707.3</v>
       </c>
       <c r="L34" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M34" t="s">
+        <v>16</v>
+      </c>
+      <c r="N34">
+        <v>20181295</v>
+      </c>
+      <c r="O34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1713,7 +2031,7 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D35">
         <v>97</v>
@@ -1740,10 +2058,19 @@
         <v>707.3</v>
       </c>
       <c r="L35" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M35" t="s">
+        <v>16</v>
+      </c>
+      <c r="N35">
+        <v>20181295</v>
+      </c>
+      <c r="O35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1751,7 +2078,7 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D36">
         <v>97</v>
@@ -1778,10 +2105,19 @@
         <v>707.3</v>
       </c>
       <c r="L36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M36" t="s">
+        <v>16</v>
+      </c>
+      <c r="N36">
+        <v>20181295</v>
+      </c>
+      <c r="O36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1789,7 +2125,7 @@
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D37">
         <v>97</v>
@@ -1816,10 +2152,19 @@
         <v>707.3</v>
       </c>
       <c r="L37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M37" t="s">
+        <v>16</v>
+      </c>
+      <c r="N37">
+        <v>20181295</v>
+      </c>
+      <c r="O37">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1827,7 +2172,7 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D38">
         <v>97</v>
@@ -1854,10 +2199,19 @@
         <v>707.3</v>
       </c>
       <c r="L38" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M38" t="s">
+        <v>16</v>
+      </c>
+      <c r="N38">
+        <v>20181295</v>
+      </c>
+      <c r="O38">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1865,7 +2219,7 @@
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D39">
         <v>97</v>
@@ -1892,10 +2246,19 @@
         <v>707.3</v>
       </c>
       <c r="L39" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M39" t="s">
+        <v>16</v>
+      </c>
+      <c r="N39">
+        <v>20181295</v>
+      </c>
+      <c r="O39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1903,7 +2266,7 @@
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D40">
         <v>97</v>
@@ -1930,10 +2293,19 @@
         <v>707.3</v>
       </c>
       <c r="L40" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M40" t="s">
+        <v>16</v>
+      </c>
+      <c r="N40">
+        <v>20181295</v>
+      </c>
+      <c r="O40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1941,7 +2313,7 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D41">
         <v>97</v>
@@ -1968,10 +2340,19 @@
         <v>707.3</v>
       </c>
       <c r="L41" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M41" t="s">
+        <v>16</v>
+      </c>
+      <c r="N41">
+        <v>20181295</v>
+      </c>
+      <c r="O41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1979,7 +2360,7 @@
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D42">
         <v>97</v>
@@ -2006,10 +2387,19 @@
         <v>707.3</v>
       </c>
       <c r="L42" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M42" t="s">
+        <v>16</v>
+      </c>
+      <c r="N42">
+        <v>20181295</v>
+      </c>
+      <c r="O42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2017,7 +2407,7 @@
         <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D43">
         <v>97</v>
@@ -2044,10 +2434,19 @@
         <v>707.3</v>
       </c>
       <c r="L43" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M43" t="s">
+        <v>16</v>
+      </c>
+      <c r="N43">
+        <v>20181295</v>
+      </c>
+      <c r="O43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2055,7 +2454,7 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D44">
         <v>97</v>
@@ -2082,10 +2481,19 @@
         <v>707.3</v>
       </c>
       <c r="L44" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12">
+        <v>15</v>
+      </c>
+      <c r="M44" t="s">
+        <v>16</v>
+      </c>
+      <c r="N44">
+        <v>20181295</v>
+      </c>
+      <c r="O44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2093,7 +2501,7 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D45">
         <v>97</v>
@@ -2120,7 +2528,16 @@
         <v>707.3</v>
       </c>
       <c r="L45" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="M45" t="s">
+        <v>16</v>
+      </c>
+      <c r="N45">
+        <v>20181295</v>
+      </c>
+      <c r="O45">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>